<commit_message>
Added Select factors for B20
</commit_message>
<xml_diff>
--- a/examples/02_annuities_in_payment/portfolio/portfolio_annuity_small.xlsx
+++ b/examples/02_annuities_in_payment/portfolio/portfolio_annuity_small.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Oracle\PyProtolinc\examples\02_annuities_in_payment\portfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B85D35F4-C545-4793-8CC7-965EEEBFD172}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7F29011-03EC-4617-AB19-DB01438D0FE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-420" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-26730" yWindow="645" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -543,7 +543,7 @@
         <v>0</v>
       </c>
       <c r="L2" s="1">
-        <v>44562</v>
+        <v>44561</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
yearly annuity product demo
</commit_message>
<xml_diff>
--- a/examples/02_annuities_in_payment/portfolio/portfolio_annuity_small.xlsx
+++ b/examples/02_annuities_in_payment/portfolio/portfolio_annuity_small.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Oracle\PyProtolinc\examples\02_annuities_in_payment\portfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7F29011-03EC-4617-AB19-DB01438D0FE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06E18179-E58A-47B5-8797-4D9895995380}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26730" yWindow="645" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -458,22 +458,22 @@
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -511,7 +511,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>44561</v>
       </c>
@@ -546,12 +546,13 @@
         <v>44561</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
+      <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>

</xml_diff>